<commit_message>
send email with post ok
</commit_message>
<xml_diff>
--- a/Amet_data.xlsx
+++ b/Amet_data.xlsx
@@ -1723,7 +1723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1843,6 +1843,78 @@
       </c>
       <c r="H3" t="n">
         <v>1678765408280</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Erneto</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Socio</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>kuva5008@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>31626117235</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Ven</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Beautiful work. I love it</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Alberto</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>El Miloitar</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>kuva5008@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>31626117235</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Ven</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Beautiful work. I love it</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>3333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>